<commit_message>
data cleaning, round 2
</commit_message>
<xml_diff>
--- a/Resources/survey_results_1.xlsx
+++ b/Resources/survey_results_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pam/class/HW/23 Project4 - Veggie/veggie-tales/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041F58A7-F00F-3248-A07F-F0F95EF79EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8384A581-8FD1-2643-B40F-080D0F0EF7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="49720" yWindow="-4400" windowWidth="36980" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="849">
   <si>
     <t>ID</t>
   </si>
@@ -820,9 +820,6 @@
     <t>Sauteed;Boiled;</t>
   </si>
   <si>
-    <t xml:space="preserve">Bananas </t>
-  </si>
-  <si>
     <t>Chicago PD</t>
   </si>
   <si>
@@ -2446,9 +2443,6 @@
     <t>Corn;Broccoli;</t>
   </si>
   <si>
-    <t xml:space="preserve">Blueberry </t>
-  </si>
-  <si>
     <t xml:space="preserve">Seinfeld </t>
   </si>
   <si>
@@ -2515,9 +2509,6 @@
     <t xml:space="preserve">Blueberries, cherries, strawberries </t>
   </si>
   <si>
-    <t xml:space="preserve">Banana, watermelon, apple </t>
-  </si>
-  <si>
     <t>Watermelon, Strawberries, Banana</t>
   </si>
   <si>
@@ -2576,6 +2567,12 @@
   </si>
   <si>
     <t>Bananna's, apples, oranges</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Banana, watermelon, apple</t>
   </si>
 </sst>
 </file>
@@ -2583,7 +2580,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -2623,7 +2620,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -2674,10 +2671,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3020,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L146" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q178" sqref="Q178"/>
+    <sheetView tabSelected="1" topLeftCell="L36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3180,7 +3177,7 @@
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -3474,7 +3471,7 @@
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3572,7 +3569,7 @@
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -3621,7 +3618,7 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3719,7 +3716,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3964,7 +3961,7 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -4503,7 +4500,7 @@
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -4993,7 +4990,7 @@
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -5091,7 +5088,7 @@
       </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -5336,7 +5333,7 @@
       </c>
       <c r="P47" s="2"/>
       <c r="Q47" s="2" t="s">
-        <v>264</v>
+        <v>513</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -5366,26 +5363,26 @@
         <v>21</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L48" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="M48" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>222</v>
       </c>
       <c r="P48" s="2"/>
       <c r="Q48" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -5415,26 +5412,26 @@
         <v>21</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L49" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>172</v>
       </c>
       <c r="P49" s="2"/>
       <c r="Q49" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
@@ -5464,26 +5461,26 @@
         <v>21</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L50" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="M50" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="N50" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P50" s="2"/>
       <c r="Q50" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -5513,26 +5510,26 @@
         <v>21</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L51" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="M51" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="N51" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="N51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
@@ -5562,26 +5559,26 @@
         <v>21</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>75</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -5611,13 +5608,13 @@
         <v>21</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>163</v>
@@ -5630,7 +5627,7 @@
       </c>
       <c r="P53" s="2"/>
       <c r="Q53" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
@@ -5660,16 +5657,16 @@
         <v>21</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>126</v>
@@ -5679,7 +5676,7 @@
       </c>
       <c r="P54" s="2"/>
       <c r="Q54" s="2" t="s">
-        <v>829</v>
+        <v>848</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -5709,26 +5706,26 @@
         <v>21</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L55" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="M55" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="N55" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>70</v>
       </c>
       <c r="P55" s="2"/>
       <c r="Q55" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -5746,38 +5743,38 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L56" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M56" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>243</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P56" s="2"/>
       <c r="Q56" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -5807,26 +5804,26 @@
         <v>21</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="N57" s="2" t="s">
+      <c r="O57" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="P57" s="2"/>
       <c r="Q57" s="2" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -5862,20 +5859,20 @@
         <v>46</v>
       </c>
       <c r="L58" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="M58" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="N58" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>193</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" s="2" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -5905,26 +5902,26 @@
         <v>21</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>251</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>222</v>
       </c>
       <c r="P59" s="2"/>
       <c r="Q59" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -5954,26 +5951,26 @@
         <v>21</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L60" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M60" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="N60" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>122</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6009,20 +6006,20 @@
         <v>38</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>135</v>
       </c>
       <c r="N61" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="O61" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
@@ -6046,32 +6043,32 @@
         <v>19</v>
       </c>
       <c r="H62" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L62" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="M62" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="M62" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="N62" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6101,26 +6098,26 @@
         <v>21</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="M63" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="M63" s="2" t="s">
+      <c r="N63" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="N63" s="2" t="s">
+      <c r="O63" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
@@ -6144,19 +6141,19 @@
         <v>19</v>
       </c>
       <c r="H64" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M64" s="2" t="s">
         <v>126</v>
@@ -6169,7 +6166,7 @@
       </c>
       <c r="P64" s="2"/>
       <c r="Q64" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6199,26 +6196,26 @@
         <v>21</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L65" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="N65" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P65" s="2"/>
       <c r="Q65" s="2" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -6248,26 +6245,26 @@
         <v>21</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L66" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M66" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="M66" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="N66" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P66" s="2"/>
       <c r="Q66" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
@@ -6297,7 +6294,7 @@
         <v>21</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>46</v>
@@ -6306,7 +6303,7 @@
         <v>139</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>160</v>
@@ -6316,7 +6313,7 @@
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" s="2" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -6352,20 +6349,20 @@
         <v>32</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>135</v>
       </c>
       <c r="N68" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="O68" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="O68" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -6395,26 +6392,26 @@
         <v>21</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L69" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="O69" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="M69" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="N69" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="O69" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
@@ -6444,26 +6441,26 @@
         <v>21</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L70" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="M70" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="M70" s="2" t="s">
+      <c r="N70" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="O70" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -6493,26 +6490,26 @@
         <v>21</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L71" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="M71" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="M71" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -6542,16 +6539,16 @@
         <v>21</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L72" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="M72" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>198</v>
@@ -6561,7 +6558,7 @@
       </c>
       <c r="P72" s="2"/>
       <c r="Q72" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
@@ -6591,26 +6588,26 @@
         <v>21</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L73" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="M73" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="N73" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="N73" s="2" t="s">
+      <c r="O73" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="P73" s="2"/>
       <c r="Q73" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
@@ -6640,26 +6637,26 @@
         <v>21</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M74" s="2" t="s">
         <v>188</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P74" s="2"/>
       <c r="Q74" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -6689,26 +6686,26 @@
         <v>21</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L75" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M75" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="N75" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="N75" s="2" t="s">
+      <c r="O75" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="P75" s="2"/>
       <c r="Q75" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -6738,26 +6735,26 @@
         <v>21</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L76" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="M76" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>135</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P76" s="2"/>
       <c r="Q76" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -6787,26 +6784,26 @@
         <v>21</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L77" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="N77" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>172</v>
       </c>
       <c r="P77" s="2"/>
       <c r="Q77" s="2" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -6836,26 +6833,26 @@
         <v>21</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O78" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P78" s="2"/>
       <c r="Q78" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -6885,26 +6882,26 @@
         <v>21</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M79" s="2" t="s">
         <v>153</v>
       </c>
       <c r="N79" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="O79" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="P79" s="2"/>
       <c r="Q79" s="2" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
@@ -6934,26 +6931,26 @@
         <v>21</v>
       </c>
       <c r="J80" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="K80" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O80" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="P80" s="2"/>
       <c r="Q80" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -6983,26 +6980,26 @@
         <v>21</v>
       </c>
       <c r="J81" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L81" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="K81" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="L81" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="O81" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="O81" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="P81" s="2"/>
       <c r="Q81" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
@@ -7032,13 +7029,13 @@
         <v>21</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>135</v>
@@ -7051,7 +7048,7 @@
       </c>
       <c r="P82" s="2"/>
       <c r="Q82" s="2" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -7081,26 +7078,26 @@
         <v>21</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L83" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="M83" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="N83" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="N83" s="2" t="s">
+      <c r="O83" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="O83" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="P83" s="2"/>
       <c r="Q83" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -7130,26 +7127,26 @@
         <v>21</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L84" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="M84" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="M84" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="N84" s="2" t="s">
         <v>216</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="P84" s="2"/>
       <c r="Q84" s="2" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -7185,10 +7182,10 @@
         <v>46</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>62</v>
@@ -7198,7 +7195,7 @@
       </c>
       <c r="P85" s="2"/>
       <c r="Q85" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -7228,26 +7225,26 @@
         <v>100</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L86" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="M86" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="M86" s="2" t="s">
+      <c r="N86" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="N86" s="2" t="s">
+      <c r="O86" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="P86" s="2"/>
       <c r="Q86" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -7283,20 +7280,20 @@
         <v>32</v>
       </c>
       <c r="L87" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="M87" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="M87" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="N87" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>259</v>
       </c>
       <c r="P87" s="2"/>
       <c r="Q87" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -7326,26 +7323,26 @@
         <v>100</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>163</v>
       </c>
       <c r="N88" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="O88" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="O88" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="P88" s="2"/>
       <c r="Q88" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -7381,20 +7378,20 @@
         <v>46</v>
       </c>
       <c r="L89" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="M89" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="M89" s="2" t="s">
-        <v>447</v>
-      </c>
       <c r="N89" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P89" s="2"/>
       <c r="Q89" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -7424,26 +7421,26 @@
         <v>21</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L90" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="M90" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="M90" s="2" t="s">
+      <c r="N90" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="N90" s="2" t="s">
+      <c r="O90" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="O90" s="2" t="s">
-        <v>452</v>
       </c>
       <c r="P90" s="2"/>
       <c r="Q90" s="2" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -7473,26 +7470,26 @@
         <v>21</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L91" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="M91" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="M91" s="2" t="s">
+      <c r="N91" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="N91" s="2" t="s">
+      <c r="O91" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="O91" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="P91" s="2"/>
       <c r="Q91" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -7522,26 +7519,26 @@
         <v>21</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>159</v>
       </c>
       <c r="N92" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="O92" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="O92" s="2" t="s">
-        <v>462</v>
       </c>
       <c r="P92" s="2"/>
       <c r="Q92" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
@@ -7571,26 +7568,26 @@
         <v>21</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="M93" s="2" t="s">
         <v>140</v>
       </c>
       <c r="N93" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="O93" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="O93" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="P93" s="2"/>
       <c r="Q93" s="2" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
@@ -7626,20 +7623,20 @@
         <v>32</v>
       </c>
       <c r="L94" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="N94" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="M94" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="N94" s="2" t="s">
+      <c r="O94" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="P94" s="2"/>
       <c r="Q94" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
@@ -7669,26 +7666,26 @@
         <v>21</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L95" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="M95" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="M95" s="2" t="s">
+      <c r="N95" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="N95" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P95" s="2"/>
       <c r="Q95" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
@@ -7718,26 +7715,26 @@
         <v>21</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L96" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="M96" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="M96" s="2" t="s">
+      <c r="N96" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="N96" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>27</v>
       </c>
       <c r="P96" s="2"/>
       <c r="Q96" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
@@ -7764,29 +7761,29 @@
         <v>20</v>
       </c>
       <c r="I97" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="J97" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>482</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L97" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="M97" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="M97" s="2" t="s">
+      <c r="N97" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="N97" s="2" t="s">
+      <c r="O97" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="O97" s="2" t="s">
-        <v>486</v>
       </c>
       <c r="P97" s="2"/>
       <c r="Q97" s="2" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -7816,26 +7813,26 @@
         <v>100</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K98" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L98" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="M98" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="M98" s="2" t="s">
+      <c r="N98" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>490</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>172</v>
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -7865,26 +7862,26 @@
         <v>21</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K99" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L99" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="M99" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="M99" s="2" t="s">
+      <c r="N99" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="N99" s="2" t="s">
-        <v>494</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>172</v>
       </c>
       <c r="P99" s="2"/>
       <c r="Q99" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
@@ -7914,7 +7911,7 @@
         <v>21</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>38</v>
@@ -7926,14 +7923,14 @@
         <v>215</v>
       </c>
       <c r="N100" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="O100" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="P100" s="2"/>
       <c r="Q100" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -7963,26 +7960,26 @@
         <v>21</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L101" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="M101" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="M101" s="2" t="s">
+      <c r="N101" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="N101" s="2" t="s">
+      <c r="O101" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="O101" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="P101" s="2"/>
       <c r="Q101" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
@@ -8012,26 +8009,26 @@
         <v>21</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>171</v>
       </c>
       <c r="N102" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="O102" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="O102" s="2" t="s">
-        <v>509</v>
       </c>
       <c r="P102" s="2"/>
       <c r="Q102" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
@@ -8061,26 +8058,26 @@
         <v>21</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L103" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="M103" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="N103" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="M103" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="N103" s="2" t="s">
-        <v>513</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P103" s="2"/>
       <c r="Q103" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -8110,26 +8107,26 @@
         <v>21</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L104" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="O104" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="O104" s="2" t="s">
-        <v>517</v>
       </c>
       <c r="P104" s="2"/>
       <c r="Q104" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -8159,26 +8156,26 @@
         <v>21</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L105" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="M105" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="M105" s="2" t="s">
+      <c r="N105" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="N105" s="2" t="s">
-        <v>522</v>
-      </c>
       <c r="O105" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P105" s="2"/>
       <c r="Q105" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
@@ -8208,26 +8205,26 @@
         <v>21</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K106" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L106" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="M106" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="M106" s="2" t="s">
+      <c r="N106" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="N106" s="2" t="s">
-        <v>527</v>
-      </c>
       <c r="O106" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P106" s="2"/>
       <c r="Q106" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
@@ -8257,26 +8254,26 @@
         <v>21</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K107" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L107" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="M107" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="M107" s="2" t="s">
+      <c r="N107" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="O107" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>532</v>
       </c>
       <c r="P107" s="2"/>
       <c r="Q107" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
@@ -8306,26 +8303,26 @@
         <v>21</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P108" s="2"/>
       <c r="Q108" s="2" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
@@ -8355,26 +8352,26 @@
         <v>21</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L109" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="M109" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="M109" s="2" t="s">
+      <c r="N109" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="N109" s="2" t="s">
-        <v>539</v>
       </c>
       <c r="O109" s="2" t="s">
         <v>87</v>
       </c>
       <c r="P109" s="2"/>
       <c r="Q109" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -8404,26 +8401,26 @@
         <v>21</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K110" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L110" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="M110" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="M110" s="2" t="s">
+      <c r="N110" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="N110" s="2" t="s">
+      <c r="O110" s="2" t="s">
         <v>544</v>
-      </c>
-      <c r="O110" s="2" t="s">
-        <v>545</v>
       </c>
       <c r="P110" s="2"/>
       <c r="Q110" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
@@ -8453,26 +8450,26 @@
         <v>21</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="K111" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L111" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="M111" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="M111" s="2" t="s">
+      <c r="N111" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="N111" s="2" t="s">
+      <c r="O111" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="O111" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="P111" s="2"/>
       <c r="Q111" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
@@ -8496,32 +8493,32 @@
         <v>19</v>
       </c>
       <c r="H112" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="I112" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="J112" s="2" t="s">
         <v>554</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>555</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L112" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="M112" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="M112" s="2" t="s">
+      <c r="N112" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="N112" s="2" t="s">
+      <c r="O112" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="O112" s="2" t="s">
-        <v>559</v>
       </c>
       <c r="P112" s="2"/>
       <c r="Q112" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
@@ -8548,7 +8545,7 @@
         <v>20</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>241</v>
@@ -8557,20 +8554,20 @@
         <v>46</v>
       </c>
       <c r="L113" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="M113" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="M113" s="2" t="s">
+      <c r="N113" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="N113" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P113" s="2"/>
       <c r="Q113" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
@@ -8600,26 +8597,26 @@
         <v>21</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K114" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M114" s="2" t="s">
         <v>62</v>
       </c>
       <c r="N114" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="O114" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="O114" s="2" t="s">
-        <v>569</v>
       </c>
       <c r="P114" s="2"/>
       <c r="Q114" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
@@ -8649,26 +8646,26 @@
         <v>21</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K115" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L115" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="M115" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="M115" s="2" t="s">
+      <c r="N115" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="N115" s="2" t="s">
-        <v>574</v>
-      </c>
       <c r="O115" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P115" s="2"/>
       <c r="Q115" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
@@ -8698,26 +8695,26 @@
         <v>21</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L116" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="M116" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="M116" s="2" t="s">
-        <v>577</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>159</v>
       </c>
       <c r="O116" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="P116" s="2"/>
       <c r="Q116" s="2" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -8747,26 +8744,26 @@
         <v>21</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K117" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L117" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="M117" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="M117" s="2" t="s">
+      <c r="N117" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="N117" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="O117" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P117" s="2"/>
       <c r="Q117" s="2" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
@@ -8796,26 +8793,26 @@
         <v>21</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="K118" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M118" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P118" s="2"/>
       <c r="Q118" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -8845,26 +8842,26 @@
         <v>21</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="M119" s="2" t="s">
         <v>103</v>
       </c>
       <c r="N119" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="O119" s="2" t="s">
         <v>589</v>
-      </c>
-      <c r="O119" s="2" t="s">
-        <v>590</v>
       </c>
       <c r="P119" s="2"/>
       <c r="Q119" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
@@ -8900,20 +8897,20 @@
         <v>32</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M120" s="2" t="s">
         <v>130</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>105</v>
       </c>
       <c r="P120" s="2"/>
       <c r="Q120" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
@@ -8949,20 +8946,20 @@
         <v>38</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M121" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O121" s="2" t="s">
         <v>199</v>
       </c>
       <c r="P121" s="2"/>
       <c r="Q121" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
@@ -8992,26 +8989,26 @@
         <v>21</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L122" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="M122" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="M122" s="2" t="s">
+      <c r="N122" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="O122" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="N122" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="O122" s="2" t="s">
-        <v>600</v>
       </c>
       <c r="P122" s="2"/>
       <c r="Q122" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
@@ -9041,26 +9038,26 @@
         <v>21</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L123" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="M123" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="M123" s="2" t="s">
+      <c r="N123" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="N123" s="2" t="s">
-        <v>604</v>
-      </c>
       <c r="O123" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P123" s="2"/>
       <c r="Q123" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
@@ -9090,26 +9087,26 @@
         <v>21</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M124" s="2" t="s">
         <v>231</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="O124" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P124" s="2"/>
       <c r="Q124" s="2" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
@@ -9139,26 +9136,26 @@
         <v>21</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K125" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L125" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="M125" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="M125" s="2" t="s">
-        <v>610</v>
-      </c>
       <c r="N125" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="O125" s="2" t="s">
         <v>122</v>
       </c>
       <c r="P125" s="2"/>
       <c r="Q125" s="2" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
@@ -9188,13 +9185,13 @@
         <v>21</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K126" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="M126" s="2" t="s">
         <v>103</v>
@@ -9203,11 +9200,11 @@
         <v>49</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P126" s="2"/>
       <c r="Q126" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
@@ -9237,13 +9234,13 @@
         <v>21</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K127" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="M127" s="2" t="s">
         <v>103</v>
@@ -9256,7 +9253,7 @@
       </c>
       <c r="P127" s="2"/>
       <c r="Q127" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
@@ -9286,13 +9283,13 @@
         <v>21</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K128" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="M128" s="2" t="s">
         <v>159</v>
@@ -9305,7 +9302,7 @@
       </c>
       <c r="P128" s="2"/>
       <c r="Q128" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
@@ -9341,20 +9338,20 @@
         <v>38</v>
       </c>
       <c r="L129" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M129" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="M129" s="2" t="s">
+      <c r="N129" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O129" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="N129" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="O129" s="2" t="s">
-        <v>622</v>
       </c>
       <c r="P129" s="2"/>
       <c r="Q129" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
@@ -9390,20 +9387,20 @@
         <v>32</v>
       </c>
       <c r="L130" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="M130" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="M130" s="2" t="s">
+      <c r="N130" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="N130" s="2" t="s">
-        <v>626</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>57</v>
       </c>
       <c r="P130" s="2"/>
       <c r="Q130" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
@@ -9430,29 +9427,29 @@
         <v>20</v>
       </c>
       <c r="I131" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="J131" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="J131" s="2" t="s">
-        <v>629</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L131" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="M131" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="M131" s="2" t="s">
+      <c r="N131" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="N131" s="2" t="s">
+      <c r="O131" s="2" t="s">
         <v>632</v>
-      </c>
-      <c r="O131" s="2" t="s">
-        <v>633</v>
       </c>
       <c r="P131" s="2"/>
       <c r="Q131" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
@@ -9482,16 +9479,16 @@
         <v>21</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K132" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="M132" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="N132" s="2" t="s">
         <v>126</v>
@@ -9501,7 +9498,7 @@
       </c>
       <c r="P132" s="2"/>
       <c r="Q132" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
@@ -9537,20 +9534,20 @@
         <v>38</v>
       </c>
       <c r="L133" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="M133" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="N133" s="2" t="s">
         <v>637</v>
-      </c>
-      <c r="M133" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="N133" s="2" t="s">
-        <v>638</v>
       </c>
       <c r="O133" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P133" s="2"/>
       <c r="Q133" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
@@ -9577,29 +9574,29 @@
         <v>20</v>
       </c>
       <c r="I134" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="J134" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>641</v>
       </c>
       <c r="K134" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L134" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="M134" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="N134" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="M134" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="N134" s="2" t="s">
-        <v>643</v>
-      </c>
       <c r="O134" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P134" s="2"/>
       <c r="Q134" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
@@ -9629,26 +9626,26 @@
         <v>21</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K135" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="M135" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N135" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="O135" s="2" t="s">
         <v>647</v>
-      </c>
-      <c r="O135" s="2" t="s">
-        <v>648</v>
       </c>
       <c r="P135" s="2"/>
       <c r="Q135" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
@@ -9675,29 +9672,29 @@
         <v>30</v>
       </c>
       <c r="I136" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="J136" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="J136" s="2" t="s">
+      <c r="K136" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L136" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="K136" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="L136" s="2" t="s">
+      <c r="M136" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="M136" s="2" t="s">
+      <c r="N136" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="N136" s="2" t="s">
+      <c r="O136" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="O136" s="2" t="s">
-        <v>655</v>
       </c>
       <c r="P136" s="2"/>
       <c r="Q136" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
@@ -9733,20 +9730,20 @@
         <v>38</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M137" s="2" t="s">
         <v>103</v>
       </c>
       <c r="N137" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O137" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="P137" s="2"/>
       <c r="Q137" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
@@ -9776,26 +9773,26 @@
         <v>21</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K138" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L138" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="M138" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N138" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O138" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P138" s="2"/>
       <c r="Q138" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
@@ -9825,26 +9822,26 @@
         <v>21</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L139" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="M139" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="M139" s="2" t="s">
+      <c r="N139" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>666</v>
       </c>
       <c r="O139" s="2" t="s">
         <v>172</v>
       </c>
       <c r="P139" s="2"/>
       <c r="Q139" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
@@ -9874,26 +9871,26 @@
         <v>21</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L140" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="M140" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="M140" s="2" t="s">
+      <c r="N140" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="N140" s="2" t="s">
+      <c r="O140" s="2" t="s">
         <v>671</v>
-      </c>
-      <c r="O140" s="2" t="s">
-        <v>672</v>
       </c>
       <c r="P140" s="2"/>
       <c r="Q140" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
@@ -9929,20 +9926,20 @@
         <v>38</v>
       </c>
       <c r="L141" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="M141" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="M141" s="2" t="s">
+      <c r="N141" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="N141" s="2" t="s">
+      <c r="O141" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="O141" s="2" t="s">
-        <v>677</v>
       </c>
       <c r="P141" s="2"/>
       <c r="Q141" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
@@ -9972,26 +9969,26 @@
         <v>21</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L142" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="M142" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="M142" s="2" t="s">
+      <c r="N142" s="2" t="s">
         <v>681</v>
-      </c>
-      <c r="N142" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="O142" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P142" s="2"/>
       <c r="Q142" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
@@ -10027,20 +10024,20 @@
         <v>38</v>
       </c>
       <c r="L143" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="M143" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="M143" s="2" t="s">
+      <c r="N143" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="O143" s="2" t="s">
         <v>685</v>
-      </c>
-      <c r="N143" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="O143" s="2" t="s">
-        <v>686</v>
       </c>
       <c r="P143" s="2"/>
       <c r="Q143" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
@@ -10058,7 +10055,7 @@
       </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>65</v>
@@ -10070,26 +10067,26 @@
         <v>21</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L144" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="M144" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="M144" s="2" t="s">
-        <v>691</v>
-      </c>
       <c r="N144" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="O144" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P144" s="2"/>
       <c r="Q144" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
@@ -10119,26 +10116,26 @@
         <v>21</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="M145" s="2" t="s">
         <v>109</v>
       </c>
       <c r="N145" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O145" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="P145" s="2"/>
       <c r="Q145" s="2" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
@@ -10168,26 +10165,26 @@
         <v>21</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="K146" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L146" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="M146" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="M146" s="2" t="s">
+      <c r="N146" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="O146" s="2" t="s">
         <v>698</v>
-      </c>
-      <c r="N146" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="O146" s="2" t="s">
-        <v>699</v>
       </c>
       <c r="P146" s="2"/>
       <c r="Q146" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -10217,26 +10214,26 @@
         <v>21</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K147" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L147" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="M147" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="N147" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="O147" s="2" t="s">
         <v>701</v>
-      </c>
-      <c r="M147" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="N147" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="O147" s="2" t="s">
-        <v>702</v>
       </c>
       <c r="P147" s="2"/>
       <c r="Q147" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
@@ -10266,26 +10263,26 @@
         <v>21</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L148" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="M148" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="M148" s="2" t="s">
+      <c r="N148" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="N148" s="2" t="s">
+      <c r="O148" s="2" t="s">
         <v>707</v>
-      </c>
-      <c r="O148" s="2" t="s">
-        <v>708</v>
       </c>
       <c r="P148" s="2"/>
       <c r="Q148" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -10315,26 +10312,26 @@
         <v>21</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K149" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M149" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N149" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O149" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P149" s="2"/>
       <c r="Q149" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
@@ -10364,26 +10361,26 @@
         <v>21</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K150" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L150" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="M150" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="M150" s="2" t="s">
+      <c r="N150" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="O150" s="2" t="s">
         <v>715</v>
-      </c>
-      <c r="N150" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="O150" s="2" t="s">
-        <v>716</v>
       </c>
       <c r="P150" s="2"/>
       <c r="Q150" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
@@ -10413,26 +10410,26 @@
         <v>21</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K151" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L151" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="M151" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="M151" s="2" t="s">
-        <v>719</v>
-      </c>
       <c r="N151" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="O151" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P151" s="2"/>
       <c r="Q151" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
@@ -10462,26 +10459,26 @@
         <v>21</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K152" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L152" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="M152" s="2" t="s">
         <v>722</v>
-      </c>
-      <c r="M152" s="2" t="s">
-        <v>723</v>
       </c>
       <c r="N152" s="2" t="s">
         <v>212</v>
       </c>
       <c r="O152" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P152" s="2"/>
       <c r="Q152" s="2" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
@@ -10508,29 +10505,29 @@
         <v>233</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L153" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="M153" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="M153" s="2" t="s">
+      <c r="N153" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="N153" s="2" t="s">
-        <v>727</v>
-      </c>
       <c r="O153" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="P153" s="2"/>
       <c r="Q153" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
@@ -10557,7 +10554,7 @@
         <v>20</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J154" s="2" t="s">
         <v>124</v>
@@ -10566,20 +10563,20 @@
         <v>46</v>
       </c>
       <c r="L154" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="M154" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="N154" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="M154" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="N154" s="2" t="s">
-        <v>730</v>
       </c>
       <c r="O154" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P154" s="2"/>
       <c r="Q154" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -10606,16 +10603,16 @@
         <v>20</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="K155" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="M155" s="2" t="s">
         <v>189</v>
@@ -10624,11 +10621,11 @@
         <v>189</v>
       </c>
       <c r="O155" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P155" s="2"/>
       <c r="Q155" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
@@ -10658,26 +10655,26 @@
         <v>21</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K156" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L156" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="N156" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="M156" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="N156" s="2" t="s">
+      <c r="O156" s="2" t="s">
         <v>736</v>
-      </c>
-      <c r="O156" s="2" t="s">
-        <v>737</v>
       </c>
       <c r="P156" s="2"/>
       <c r="Q156" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
@@ -10707,26 +10704,26 @@
         <v>21</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K157" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L157" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="M157" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="N157" s="2" t="s">
         <v>740</v>
-      </c>
-      <c r="M157" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="N157" s="2" t="s">
-        <v>741</v>
       </c>
       <c r="O157" s="2" t="s">
         <v>87</v>
       </c>
       <c r="P157" s="2"/>
       <c r="Q157" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
@@ -10756,26 +10753,26 @@
         <v>21</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L158" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="M158" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="N158" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="M158" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="N158" s="2" t="s">
+      <c r="O158" s="2" t="s">
         <v>745</v>
-      </c>
-      <c r="O158" s="2" t="s">
-        <v>746</v>
       </c>
       <c r="P158" s="2"/>
       <c r="Q158" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
@@ -10805,26 +10802,26 @@
         <v>21</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="K159" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L159" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="N159" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="M159" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="N159" s="2" t="s">
-        <v>750</v>
-      </c>
       <c r="O159" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P159" s="2"/>
       <c r="Q159" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
@@ -10860,16 +10857,16 @@
         <v>38</v>
       </c>
       <c r="L160" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="M160" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="M160" s="2" t="s">
+      <c r="N160" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O160" s="2" t="s">
         <v>753</v>
-      </c>
-      <c r="N160" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="O160" s="2" t="s">
-        <v>754</v>
       </c>
       <c r="P160" s="2"/>
       <c r="Q160" s="2" t="s">
@@ -10903,26 +10900,26 @@
         <v>21</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="K161" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L161" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="M161" s="2" t="s">
         <v>90</v>
       </c>
       <c r="N161" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O161" s="2" t="s">
         <v>111</v>
       </c>
       <c r="P161" s="2"/>
       <c r="Q161" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
@@ -10952,26 +10949,26 @@
         <v>21</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L162" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="M162" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="M162" s="2" t="s">
+      <c r="N162" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="N162" s="2" t="s">
+      <c r="O162" s="2" t="s">
         <v>762</v>
-      </c>
-      <c r="O162" s="2" t="s">
-        <v>763</v>
       </c>
       <c r="P162" s="2"/>
       <c r="Q162" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
@@ -10998,7 +10995,7 @@
         <v>20</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J163" s="2" t="s">
         <v>119</v>
@@ -11007,20 +11004,20 @@
         <v>38</v>
       </c>
       <c r="L163" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="N163" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="P163" s="2"/>
       <c r="Q163" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
@@ -11056,20 +11053,20 @@
         <v>32</v>
       </c>
       <c r="L164" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="M164" s="2" t="s">
         <v>768</v>
-      </c>
-      <c r="M164" s="2" t="s">
-        <v>769</v>
       </c>
       <c r="N164" s="2" t="s">
         <v>104</v>
       </c>
       <c r="O164" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="P164" s="2"/>
       <c r="Q164" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
@@ -11105,20 +11102,20 @@
         <v>32</v>
       </c>
       <c r="L165" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="M165" s="2" t="s">
         <v>49</v>
       </c>
       <c r="N165" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="O165" s="2" t="s">
         <v>773</v>
-      </c>
-      <c r="O165" s="2" t="s">
-        <v>774</v>
       </c>
       <c r="P165" s="2"/>
       <c r="Q165" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
@@ -11148,26 +11145,26 @@
         <v>21</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L166" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="M166" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="M166" s="2" t="s">
-        <v>778</v>
-      </c>
       <c r="N166" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="O166" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="P166" s="2"/>
       <c r="Q166" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
@@ -11194,29 +11191,29 @@
         <v>20</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K167" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L167" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="M167" s="2" t="s">
         <v>781</v>
       </c>
-      <c r="M167" s="2" t="s">
+      <c r="N167" s="2" t="s">
         <v>782</v>
       </c>
-      <c r="N167" s="2" t="s">
+      <c r="O167" s="2" t="s">
         <v>783</v>
-      </c>
-      <c r="O167" s="2" t="s">
-        <v>784</v>
       </c>
       <c r="P167" s="2"/>
       <c r="Q167" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
@@ -11246,26 +11243,26 @@
         <v>21</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L168" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="M168" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="M168" s="2" t="s">
+      <c r="N168" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="N168" s="2" t="s">
-        <v>789</v>
-      </c>
       <c r="O168" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P168" s="2"/>
       <c r="Q168" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
@@ -11295,26 +11292,26 @@
         <v>21</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L169" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="M169" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N169" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="O169" s="2" t="s">
         <v>793</v>
-      </c>
-      <c r="O169" s="2" t="s">
-        <v>794</v>
       </c>
       <c r="P169" s="2"/>
       <c r="Q169" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
@@ -11344,19 +11341,19 @@
         <v>21</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K170" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="M170" s="2" t="s">
         <v>134</v>
       </c>
       <c r="N170" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O170" s="2" t="s">
         <v>111</v>
@@ -11393,26 +11390,26 @@
         <v>21</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="K171" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L171" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M171" s="2" t="s">
         <v>798</v>
       </c>
-      <c r="M171" s="2" t="s">
+      <c r="N171" s="2" t="s">
         <v>799</v>
       </c>
-      <c r="N171" s="2" t="s">
+      <c r="O171" s="2" t="s">
         <v>800</v>
-      </c>
-      <c r="O171" s="2" t="s">
-        <v>801</v>
       </c>
       <c r="P171" s="2"/>
       <c r="Q171" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
@@ -11442,26 +11439,26 @@
         <v>21</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K172" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L172" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="M172" s="2" t="s">
         <v>804</v>
       </c>
-      <c r="M172" s="2" t="s">
-        <v>805</v>
-      </c>
       <c r="N172" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O172" s="2" t="s">
         <v>76</v>
       </c>
       <c r="P172" s="2"/>
       <c r="Q172" s="2" t="s">
-        <v>806</v>
+        <v>847</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
@@ -11491,7 +11488,7 @@
         <v>21</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="K173" s="2" t="s">
         <v>32</v>
@@ -11500,7 +11497,7 @@
         <v>49</v>
       </c>
       <c r="M173" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N173" s="2" t="s">
         <v>189</v>
@@ -11510,7 +11507,7 @@
       </c>
       <c r="P173" s="2"/>
       <c r="Q173" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
@@ -11540,13 +11537,13 @@
         <v>21</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="K174" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="L174" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="M174" s="2" t="s">
         <v>139</v>
@@ -11559,7 +11556,7 @@
       </c>
       <c r="P174" s="2"/>
       <c r="Q174" s="2" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
@@ -11589,26 +11586,26 @@
         <v>21</v>
       </c>
       <c r="J175" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="K175" s="2" t="s">
         <v>32</v>
       </c>
       <c r="L175" s="2" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="M175" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="N175" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O175" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P175" s="2"/>
       <c r="Q175" s="2" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -11638,26 +11635,26 @@
         <v>21</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L176" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="M176" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="N176" s="2" t="s">
         <v>815</v>
-      </c>
-      <c r="M176" s="2" t="s">
-        <v>816</v>
-      </c>
-      <c r="N176" s="2" t="s">
-        <v>817</v>
       </c>
       <c r="O176" s="2" t="s">
         <v>193</v>
       </c>
       <c r="P176" s="2"/>
       <c r="Q176" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data cleaing, round 2
</commit_message>
<xml_diff>
--- a/Resources/survey_results_1.xlsx
+++ b/Resources/survey_results_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pam/class/HW/23 Project4 - Veggie/veggie-tales/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFFB972-4A92-7448-BB78-A6E1374F6DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588076B8-82E0-AC40-AA2A-22BB0089E1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47000" yWindow="-4460" windowWidth="36980" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50720" yWindow="-4600" windowWidth="36980" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -796,9 +796,6 @@
     <t>Chicago PD</t>
   </si>
   <si>
-    <t>Corn;Lettuce (any kind);Spinach;Squash;Brussel sprouts ;</t>
-  </si>
-  <si>
     <t>Lettuce (any kind);Spinach;Corn;</t>
   </si>
   <si>
@@ -2563,10 +2560,13 @@
     <t>Broccoli;Carrots;Lettuce (any kind);Bell pepper;onions ;</t>
   </si>
   <si>
-    <t>Corn;Green Beans;Asparagus;Brussel Sprouts ;Lettuce (any kind);</t>
-  </si>
-  <si>
     <t>Broccoli;Corn;Lettuce (any kind);Onions;tomatoes;</t>
+  </si>
+  <si>
+    <t>Corn;Lettuce (any kind);Spinach;Squash;Brussel sprouts;</t>
+  </si>
+  <si>
+    <t>Corn;Green Beans;Asparagus;Brussel Sprouts;Lettuce (any kind);</t>
   </si>
 </sst>
 </file>
@@ -3011,7 +3011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H60" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G97" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L176"/>
     </sheetView>
   </sheetViews>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -3612,7 +3612,7 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -4543,7 +4543,7 @@
       </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -4775,7 +4775,7 @@
         <v>31</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>205</v>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="P42" s="2"/>
       <c r="Q42" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -5118,7 +5118,7 @@
         <v>37</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>238</v>
@@ -5131,7 +5131,7 @@
       </c>
       <c r="P43" s="2"/>
       <c r="Q43" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="P46" s="2"/>
       <c r="Q46" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -5327,7 +5327,7 @@
       </c>
       <c r="P47" s="2"/>
       <c r="Q47" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -5363,20 +5363,20 @@
         <v>37</v>
       </c>
       <c r="L48" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="M48" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>216</v>
       </c>
       <c r="P48" s="2"/>
       <c r="Q48" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -5406,26 +5406,26 @@
         <v>21</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="M49" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="N49" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>169</v>
       </c>
       <c r="P49" s="2"/>
       <c r="Q49" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
@@ -5455,26 +5455,26 @@
         <v>21</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="M50" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="N50" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P50" s="2"/>
       <c r="Q50" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -5504,26 +5504,26 @@
         <v>21</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L51" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="M51" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="N51" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="N51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="P51" s="2"/>
       <c r="Q51" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
@@ -5553,26 +5553,26 @@
         <v>21</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>73</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -5602,13 +5602,13 @@
         <v>21</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>160</v>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="P53" s="2"/>
       <c r="Q53" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
@@ -5651,16 +5651,16 @@
         <v>21</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>124</v>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="P54" s="2"/>
       <c r="Q54" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -5700,26 +5700,26 @@
         <v>21</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L55" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="M55" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="M55" s="2" t="s">
+      <c r="N55" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>68</v>
       </c>
       <c r="P55" s="2"/>
       <c r="Q55" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -5737,38 +5737,38 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L56" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="M56" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>237</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P56" s="2"/>
       <c r="Q56" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -5798,26 +5798,26 @@
         <v>21</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M57" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="N57" s="2" t="s">
+      <c r="O57" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="P57" s="2"/>
       <c r="Q57" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -5853,20 +5853,20 @@
         <v>45</v>
       </c>
       <c r="L58" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="M58" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="N58" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>188</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
@@ -5896,26 +5896,26 @@
         <v>21</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M59" s="2" t="s">
         <v>243</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>216</v>
       </c>
       <c r="P59" s="2"/>
       <c r="Q59" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -5945,26 +5945,26 @@
         <v>21</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L60" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="M60" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="N60" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="N60" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="O60" s="2" t="s">
         <v>120</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6000,20 +6000,20 @@
         <v>37</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M61" s="2" t="s">
         <v>133</v>
       </c>
       <c r="N61" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="O61" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
@@ -6037,32 +6037,32 @@
         <v>19</v>
       </c>
       <c r="H62" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L62" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="M62" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="M62" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="N62" s="2" t="s">
+      <c r="O62" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6092,26 +6092,26 @@
         <v>21</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L63" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="M63" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="M63" s="2" t="s">
+      <c r="N63" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="N63" s="2" t="s">
+      <c r="O63" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="P63" s="2"/>
       <c r="Q63" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
@@ -6135,19 +6135,19 @@
         <v>19</v>
       </c>
       <c r="H64" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M64" s="2" t="s">
         <v>124</v>
@@ -6160,7 +6160,7 @@
       </c>
       <c r="P64" s="2"/>
       <c r="Q64" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6190,26 +6190,26 @@
         <v>21</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L65" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="M65" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="M65" s="2" t="s">
+      <c r="N65" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="N65" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="O65" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P65" s="2"/>
       <c r="Q65" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -6239,26 +6239,26 @@
         <v>21</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L66" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="M66" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="M66" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="N66" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O66" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P66" s="2"/>
       <c r="Q66" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
@@ -6288,7 +6288,7 @@
         <v>21</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>45</v>
@@ -6297,7 +6297,7 @@
         <v>137</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N67" s="2" t="s">
         <v>158</v>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="P67" s="2"/>
       <c r="Q67" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
@@ -6343,20 +6343,20 @@
         <v>31</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>133</v>
       </c>
       <c r="N68" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="O68" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="O68" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="P68" s="2"/>
       <c r="Q68" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
@@ -6386,26 +6386,26 @@
         <v>21</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L69" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="M69" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="O69" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="M69" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="N69" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="O69" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="P69" s="2"/>
       <c r="Q69" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
@@ -6435,26 +6435,26 @@
         <v>21</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L70" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M70" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="M70" s="2" t="s">
+      <c r="N70" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="O70" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
@@ -6484,26 +6484,26 @@
         <v>21</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L71" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="M71" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="M71" s="2" t="s">
+      <c r="N71" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P71" s="2"/>
       <c r="Q71" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
@@ -6533,16 +6533,16 @@
         <v>21</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L72" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="M72" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>193</v>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="P72" s="2"/>
       <c r="Q72" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
@@ -6582,26 +6582,26 @@
         <v>21</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L73" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="M73" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="M73" s="2" t="s">
+      <c r="N73" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="N73" s="2" t="s">
+      <c r="O73" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="P73" s="2"/>
       <c r="Q73" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
@@ -6631,26 +6631,26 @@
         <v>21</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M74" s="2" t="s">
         <v>184</v>
       </c>
       <c r="N74" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O74" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P74" s="2"/>
       <c r="Q74" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
@@ -6680,26 +6680,26 @@
         <v>21</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="M75" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="N75" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="N75" s="2" t="s">
+      <c r="O75" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="P75" s="2"/>
       <c r="Q75" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
@@ -6729,26 +6729,26 @@
         <v>21</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N76" s="2" t="s">
         <v>133</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="P76" s="2"/>
       <c r="Q76" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
@@ -6778,19 +6778,19 @@
         <v>21</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L77" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="M77" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="N77" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="N77" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="O77" s="2" t="s">
         <v>169</v>
@@ -6827,26 +6827,26 @@
         <v>21</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O78" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P78" s="2"/>
       <c r="Q78" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -6876,26 +6876,26 @@
         <v>21</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M79" s="2" t="s">
         <v>151</v>
       </c>
       <c r="N79" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="O79" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="P79" s="2"/>
       <c r="Q79" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
@@ -6925,26 +6925,26 @@
         <v>21</v>
       </c>
       <c r="J80" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K80" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="O80" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="N80" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="P80" s="2"/>
       <c r="Q80" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -6974,26 +6974,26 @@
         <v>21</v>
       </c>
       <c r="J81" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L81" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="K81" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="L81" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="O81" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="O81" s="2" t="s">
-        <v>394</v>
       </c>
       <c r="P81" s="2"/>
       <c r="Q81" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
@@ -7023,13 +7023,13 @@
         <v>21</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>133</v>
@@ -7042,7 +7042,7 @@
       </c>
       <c r="P82" s="2"/>
       <c r="Q82" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -7072,26 +7072,26 @@
         <v>21</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L83" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="M83" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="M83" s="2" t="s">
+      <c r="N83" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="N83" s="2" t="s">
+      <c r="O83" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="O83" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="P83" s="2"/>
       <c r="Q83" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -7121,26 +7121,26 @@
         <v>21</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L84" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="M84" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="M84" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="N84" s="2" t="s">
         <v>210</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P84" s="2"/>
       <c r="Q84" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -7176,10 +7176,10 @@
         <v>45</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>61</v>
@@ -7189,7 +7189,7 @@
       </c>
       <c r="P85" s="2"/>
       <c r="Q85" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
@@ -7219,26 +7219,26 @@
         <v>98</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L86" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="M86" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="M86" s="2" t="s">
+      <c r="N86" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="N86" s="2" t="s">
+      <c r="O86" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="P86" s="2"/>
       <c r="Q86" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
@@ -7274,20 +7274,20 @@
         <v>31</v>
       </c>
       <c r="L87" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="M87" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="M87" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="N87" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O87" s="2" t="s">
         <v>251</v>
       </c>
       <c r="P87" s="2"/>
       <c r="Q87" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -7317,26 +7317,26 @@
         <v>98</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M88" s="2" t="s">
         <v>160</v>
       </c>
       <c r="N88" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="O88" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="O88" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="P88" s="2"/>
       <c r="Q88" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -7372,20 +7372,20 @@
         <v>45</v>
       </c>
       <c r="L89" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="M89" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="M89" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="N89" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="O89" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P89" s="2"/>
       <c r="Q89" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -7415,26 +7415,26 @@
         <v>21</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L90" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="M90" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="M90" s="2" t="s">
+      <c r="N90" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="N90" s="2" t="s">
+      <c r="O90" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="O90" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="P90" s="2"/>
       <c r="Q90" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -7464,26 +7464,26 @@
         <v>21</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L91" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="M91" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="M91" s="2" t="s">
+      <c r="N91" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="N91" s="2" t="s">
+      <c r="O91" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="O91" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="P91" s="2"/>
       <c r="Q91" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -7513,26 +7513,26 @@
         <v>21</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="M92" s="2" t="s">
         <v>157</v>
       </c>
       <c r="N92" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="O92" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="O92" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="P92" s="2"/>
       <c r="Q92" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
@@ -7562,26 +7562,26 @@
         <v>21</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="M93" s="2" t="s">
         <v>138</v>
       </c>
       <c r="N93" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="O93" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="O93" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="P93" s="2"/>
       <c r="Q93" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
@@ -7617,20 +7617,20 @@
         <v>31</v>
       </c>
       <c r="L94" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="N94" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="M94" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="N94" s="2" t="s">
+      <c r="O94" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="O94" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="P94" s="2"/>
       <c r="Q94" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
@@ -7660,26 +7660,26 @@
         <v>21</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L95" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="M95" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="M95" s="2" t="s">
+      <c r="N95" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="N95" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="O95" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P95" s="2"/>
       <c r="Q95" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
@@ -7709,26 +7709,26 @@
         <v>21</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="M96" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="N96" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="N96" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="O96" s="2" t="s">
         <v>27</v>
       </c>
       <c r="P96" s="2"/>
       <c r="Q96" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
@@ -7755,29 +7755,29 @@
         <v>20</v>
       </c>
       <c r="I97" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="J97" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>454</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="M97" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="N97" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="N97" s="2" t="s">
+      <c r="O97" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="O97" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="P97" s="2"/>
       <c r="Q97" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
@@ -7807,26 +7807,26 @@
         <v>98</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K98" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L98" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="M98" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="M98" s="2" t="s">
+      <c r="N98" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="N98" s="2" t="s">
-        <v>461</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>169</v>
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -7856,26 +7856,26 @@
         <v>21</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K99" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L99" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="M99" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="M99" s="2" t="s">
+      <c r="N99" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="N99" s="2" t="s">
-        <v>464</v>
       </c>
       <c r="O99" s="2" t="s">
         <v>169</v>
       </c>
       <c r="P99" s="2"/>
       <c r="Q99" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
@@ -7905,7 +7905,7 @@
         <v>21</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>37</v>
@@ -7917,14 +7917,14 @@
         <v>209</v>
       </c>
       <c r="N100" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="O100" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="P100" s="2"/>
       <c r="Q100" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
@@ -7954,26 +7954,26 @@
         <v>21</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L101" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="M101" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="M101" s="2" t="s">
+      <c r="N101" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="N101" s="2" t="s">
+      <c r="O101" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="O101" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="P101" s="2"/>
       <c r="Q101" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
@@ -8003,26 +8003,26 @@
         <v>21</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>168</v>
       </c>
       <c r="N102" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="O102" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="O102" s="2" t="s">
-        <v>478</v>
       </c>
       <c r="P102" s="2"/>
       <c r="Q102" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
@@ -8052,26 +8052,26 @@
         <v>21</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L103" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="M103" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="N103" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="M103" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="N103" s="2" t="s">
-        <v>482</v>
       </c>
       <c r="O103" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P103" s="2"/>
       <c r="Q103" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -8101,26 +8101,26 @@
         <v>21</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P104" s="2"/>
       <c r="Q104" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
@@ -8150,26 +8150,26 @@
         <v>21</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L105" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="M105" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="M105" s="2" t="s">
+      <c r="N105" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="N105" s="2" t="s">
-        <v>489</v>
-      </c>
       <c r="O105" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P105" s="2"/>
       <c r="Q105" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
@@ -8199,26 +8199,26 @@
         <v>21</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K106" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L106" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="M106" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="M106" s="2" t="s">
+      <c r="N106" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="N106" s="2" t="s">
-        <v>494</v>
-      </c>
       <c r="O106" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P106" s="2"/>
       <c r="Q106" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
@@ -8248,26 +8248,26 @@
         <v>21</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K107" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L107" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="M107" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="M107" s="2" t="s">
+      <c r="N107" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="O107" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="N107" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="O107" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="P107" s="2"/>
       <c r="Q107" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
@@ -8297,26 +8297,26 @@
         <v>21</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M108" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P108" s="2"/>
       <c r="Q108" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
@@ -8346,26 +8346,26 @@
         <v>21</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="M109" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="N109" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="N109" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="O109" s="2" t="s">
         <v>85</v>
       </c>
       <c r="P109" s="2"/>
       <c r="Q109" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -8395,26 +8395,26 @@
         <v>21</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K110" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L110" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="M110" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="M110" s="2" t="s">
+      <c r="N110" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="N110" s="2" t="s">
+      <c r="O110" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="O110" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="P110" s="2"/>
       <c r="Q110" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
@@ -8444,26 +8444,26 @@
         <v>21</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K111" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L111" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="M111" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="M111" s="2" t="s">
+      <c r="N111" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="N111" s="2" t="s">
+      <c r="O111" s="2" t="s">
         <v>515</v>
-      </c>
-      <c r="O111" s="2" t="s">
-        <v>516</v>
       </c>
       <c r="P111" s="2"/>
       <c r="Q111" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
@@ -8487,32 +8487,32 @@
         <v>19</v>
       </c>
       <c r="H112" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="I112" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="J112" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L112" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="M112" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="M112" s="2" t="s">
+      <c r="N112" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="N112" s="2" t="s">
+      <c r="O112" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="O112" s="2" t="s">
-        <v>524</v>
       </c>
       <c r="P112" s="2"/>
       <c r="Q112" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
@@ -8539,7 +8539,7 @@
         <v>20</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J113" s="2" t="s">
         <v>235</v>
@@ -8548,20 +8548,20 @@
         <v>45</v>
       </c>
       <c r="L113" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="M113" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="M113" s="2" t="s">
+      <c r="N113" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="N113" s="2" t="s">
-        <v>528</v>
       </c>
       <c r="O113" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P113" s="2"/>
       <c r="Q113" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
@@ -8591,26 +8591,26 @@
         <v>21</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="K114" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="M114" s="2" t="s">
         <v>61</v>
       </c>
       <c r="N114" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="O114" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="O114" s="2" t="s">
-        <v>533</v>
       </c>
       <c r="P114" s="2"/>
       <c r="Q114" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.2">
@@ -8640,26 +8640,26 @@
         <v>21</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K115" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M115" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="N115" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="N115" s="2" t="s">
-        <v>537</v>
-      </c>
       <c r="O115" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P115" s="2"/>
       <c r="Q115" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
@@ -8689,26 +8689,26 @@
         <v>21</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L116" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="M116" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="M116" s="2" t="s">
-        <v>539</v>
       </c>
       <c r="N116" s="2" t="s">
         <v>157</v>
       </c>
       <c r="O116" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="P116" s="2"/>
       <c r="Q116" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
@@ -8738,26 +8738,26 @@
         <v>21</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K117" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="M117" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="N117" s="2" t="s">
         <v>542</v>
-      </c>
-      <c r="N117" s="2" t="s">
-        <v>543</v>
       </c>
       <c r="O117" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P117" s="2"/>
       <c r="Q117" s="2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
@@ -8787,26 +8787,26 @@
         <v>21</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K118" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="M118" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P118" s="2"/>
       <c r="Q118" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -8836,26 +8836,26 @@
         <v>21</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="M119" s="2" t="s">
         <v>101</v>
       </c>
       <c r="N119" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="O119" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="O119" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="P119" s="2"/>
       <c r="Q119" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
@@ -8891,20 +8891,20 @@
         <v>31</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="M120" s="2" t="s">
         <v>128</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="O120" s="2" t="s">
         <v>103</v>
       </c>
       <c r="P120" s="2"/>
       <c r="Q120" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
@@ -8940,20 +8940,20 @@
         <v>37</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="M121" s="2" t="s">
         <v>39</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O121" s="2" t="s">
         <v>194</v>
       </c>
       <c r="P121" s="2"/>
       <c r="Q121" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.2">
@@ -8983,26 +8983,26 @@
         <v>21</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L122" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="M122" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="M122" s="2" t="s">
+      <c r="N122" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="O122" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="N122" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="O122" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="P122" s="2"/>
       <c r="Q122" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
@@ -9032,26 +9032,26 @@
         <v>21</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L123" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="M123" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="M123" s="2" t="s">
+      <c r="N123" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="N123" s="2" t="s">
-        <v>563</v>
-      </c>
       <c r="O123" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P123" s="2"/>
       <c r="Q123" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">
@@ -9081,26 +9081,26 @@
         <v>21</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M124" s="2" t="s">
         <v>225</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="O124" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="P124" s="2"/>
       <c r="Q124" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
@@ -9130,26 +9130,26 @@
         <v>21</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K125" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O125" s="2" t="s">
         <v>120</v>
       </c>
       <c r="P125" s="2"/>
       <c r="Q125" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
@@ -9179,13 +9179,13 @@
         <v>21</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K126" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M126" s="2" t="s">
         <v>101</v>
@@ -9194,11 +9194,11 @@
         <v>48</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P126" s="2"/>
       <c r="Q126" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
@@ -9228,13 +9228,13 @@
         <v>21</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K127" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M127" s="2" t="s">
         <v>101</v>
@@ -9247,7 +9247,7 @@
       </c>
       <c r="P127" s="2"/>
       <c r="Q127" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
@@ -9277,13 +9277,13 @@
         <v>21</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K128" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="M128" s="2" t="s">
         <v>157</v>
@@ -9296,7 +9296,7 @@
       </c>
       <c r="P128" s="2"/>
       <c r="Q128" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
@@ -9332,20 +9332,20 @@
         <v>37</v>
       </c>
       <c r="L129" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="M129" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="M129" s="2" t="s">
+      <c r="N129" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="O129" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="N129" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="O129" s="2" t="s">
-        <v>580</v>
       </c>
       <c r="P129" s="2"/>
       <c r="Q129" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
@@ -9381,20 +9381,20 @@
         <v>31</v>
       </c>
       <c r="L130" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="M130" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="M130" s="2" t="s">
+      <c r="N130" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="N130" s="2" t="s">
-        <v>584</v>
       </c>
       <c r="O130" s="2" t="s">
         <v>56</v>
       </c>
       <c r="P130" s="2"/>
       <c r="Q130" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
@@ -9421,29 +9421,29 @@
         <v>20</v>
       </c>
       <c r="I131" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="J131" s="2" t="s">
         <v>586</v>
-      </c>
-      <c r="J131" s="2" t="s">
-        <v>587</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L131" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="M131" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="M131" s="2" t="s">
+      <c r="N131" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="N131" s="2" t="s">
+      <c r="O131" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="O131" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="P131" s="2"/>
       <c r="Q131" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
@@ -9473,16 +9473,16 @@
         <v>21</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K132" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="M132" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N132" s="2" t="s">
         <v>124</v>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="P132" s="2"/>
       <c r="Q132" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
@@ -9528,20 +9528,20 @@
         <v>37</v>
       </c>
       <c r="L133" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="M133" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="N133" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="M133" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="N133" s="2" t="s">
-        <v>596</v>
       </c>
       <c r="O133" s="2" t="s">
         <v>41</v>
       </c>
       <c r="P133" s="2"/>
       <c r="Q133" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
@@ -9568,29 +9568,29 @@
         <v>20</v>
       </c>
       <c r="I134" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="J134" s="2" t="s">
         <v>598</v>
-      </c>
-      <c r="J134" s="2" t="s">
-        <v>599</v>
       </c>
       <c r="K134" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L134" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="M134" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="N134" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="M134" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="N134" s="2" t="s">
-        <v>601</v>
-      </c>
       <c r="O134" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P134" s="2"/>
       <c r="Q134" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
@@ -9620,26 +9620,26 @@
         <v>21</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K135" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="M135" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N135" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="O135" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="O135" s="2" t="s">
-        <v>605</v>
       </c>
       <c r="P135" s="2"/>
       <c r="Q135" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
@@ -9666,29 +9666,29 @@
         <v>29</v>
       </c>
       <c r="I136" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="J136" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="J136" s="2" t="s">
+      <c r="K136" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L136" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="K136" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="L136" s="2" t="s">
+      <c r="M136" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="M136" s="2" t="s">
+      <c r="N136" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="N136" s="2" t="s">
+      <c r="O136" s="2" t="s">
         <v>611</v>
-      </c>
-      <c r="O136" s="2" t="s">
-        <v>612</v>
       </c>
       <c r="P136" s="2"/>
       <c r="Q136" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
@@ -9724,20 +9724,20 @@
         <v>37</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M137" s="2" t="s">
         <v>101</v>
       </c>
       <c r="N137" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="O137" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="P137" s="2"/>
       <c r="Q137" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
@@ -9767,26 +9767,26 @@
         <v>21</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K138" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L138" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="M138" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N138" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O138" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P138" s="2"/>
       <c r="Q138" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
@@ -9816,26 +9816,26 @@
         <v>21</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L139" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M139" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="M139" s="2" t="s">
+      <c r="N139" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="N139" s="2" t="s">
-        <v>622</v>
       </c>
       <c r="O139" s="2" t="s">
         <v>169</v>
       </c>
       <c r="P139" s="2"/>
       <c r="Q139" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
@@ -9865,26 +9865,26 @@
         <v>21</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L140" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="M140" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="M140" s="2" t="s">
+      <c r="N140" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="N140" s="2" t="s">
+      <c r="O140" s="2" t="s">
         <v>626</v>
-      </c>
-      <c r="O140" s="2" t="s">
-        <v>627</v>
       </c>
       <c r="P140" s="2"/>
       <c r="Q140" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
@@ -9920,20 +9920,20 @@
         <v>37</v>
       </c>
       <c r="L141" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="M141" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="M141" s="2" t="s">
+      <c r="N141" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="N141" s="2" t="s">
+      <c r="O141" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="O141" s="2" t="s">
-        <v>632</v>
       </c>
       <c r="P141" s="2"/>
       <c r="Q141" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
@@ -9963,26 +9963,26 @@
         <v>21</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="M142" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="N142" s="2" t="s">
         <v>634</v>
-      </c>
-      <c r="N142" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="O142" s="2" t="s">
         <v>41</v>
       </c>
       <c r="P142" s="2"/>
       <c r="Q142" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
@@ -10018,20 +10018,20 @@
         <v>37</v>
       </c>
       <c r="L143" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="M143" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="M143" s="2" t="s">
+      <c r="N143" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="O143" s="2" t="s">
         <v>637</v>
-      </c>
-      <c r="N143" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="O143" s="2" t="s">
-        <v>638</v>
       </c>
       <c r="P143" s="2"/>
       <c r="Q143" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>63</v>
@@ -10061,26 +10061,26 @@
         <v>21</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L144" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="M144" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="M144" s="2" t="s">
-        <v>643</v>
-      </c>
       <c r="N144" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="O144" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P144" s="2"/>
       <c r="Q144" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
@@ -10110,26 +10110,26 @@
         <v>21</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="M145" s="2" t="s">
         <v>107</v>
       </c>
       <c r="N145" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O145" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="P145" s="2"/>
       <c r="Q145" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
@@ -10159,26 +10159,26 @@
         <v>21</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K146" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L146" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M146" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="N146" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="O146" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="N146" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="O146" s="2" t="s">
-        <v>650</v>
       </c>
       <c r="P146" s="2"/>
       <c r="Q146" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -10208,26 +10208,26 @@
         <v>21</v>
       </c>
       <c r="J147" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K147" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L147" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="M147" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="N147" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="O147" s="2" t="s">
         <v>652</v>
-      </c>
-      <c r="M147" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="N147" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="O147" s="2" t="s">
-        <v>653</v>
       </c>
       <c r="P147" s="2"/>
       <c r="Q147" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
@@ -10257,26 +10257,26 @@
         <v>21</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L148" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="M148" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="M148" s="2" t="s">
+      <c r="N148" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="N148" s="2" t="s">
+      <c r="O148" s="2" t="s">
         <v>658</v>
-      </c>
-      <c r="O148" s="2" t="s">
-        <v>659</v>
       </c>
       <c r="P148" s="2"/>
       <c r="Q148" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -10306,26 +10306,26 @@
         <v>21</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="K149" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="M149" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N149" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O149" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P149" s="2"/>
       <c r="Q149" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
@@ -10355,26 +10355,26 @@
         <v>21</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K150" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L150" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="M150" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="M150" s="2" t="s">
+      <c r="N150" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="O150" s="2" t="s">
         <v>666</v>
-      </c>
-      <c r="N150" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="O150" s="2" t="s">
-        <v>667</v>
       </c>
       <c r="P150" s="2"/>
       <c r="Q150" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
@@ -10404,26 +10404,26 @@
         <v>21</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K151" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L151" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="M151" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="M151" s="2" t="s">
-        <v>670</v>
-      </c>
       <c r="N151" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O151" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P151" s="2"/>
       <c r="Q151" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
@@ -10453,26 +10453,26 @@
         <v>21</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K152" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="N152" s="2" t="s">
         <v>206</v>
       </c>
       <c r="O152" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P152" s="2"/>
       <c r="Q152" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
@@ -10499,29 +10499,29 @@
         <v>227</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L153" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="M153" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="M153" s="2" t="s">
+      <c r="N153" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="N153" s="2" t="s">
-        <v>677</v>
-      </c>
       <c r="O153" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="P153" s="2"/>
       <c r="Q153" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
@@ -10548,7 +10548,7 @@
         <v>20</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J154" s="2" t="s">
         <v>122</v>
@@ -10557,20 +10557,20 @@
         <v>45</v>
       </c>
       <c r="L154" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="M154" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="N154" s="2" t="s">
         <v>678</v>
-      </c>
-      <c r="M154" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="N154" s="2" t="s">
-        <v>679</v>
       </c>
       <c r="O154" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P154" s="2"/>
       <c r="Q154" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -10597,16 +10597,16 @@
         <v>20</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K155" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M155" s="2" t="s">
         <v>185</v>
@@ -10615,11 +10615,11 @@
         <v>185</v>
       </c>
       <c r="O155" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P155" s="2"/>
       <c r="Q155" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
@@ -10655,20 +10655,20 @@
         <v>31</v>
       </c>
       <c r="L156" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="M156" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="N156" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="M156" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="N156" s="2" t="s">
+      <c r="O156" s="2" t="s">
         <v>685</v>
-      </c>
-      <c r="O156" s="2" t="s">
-        <v>686</v>
       </c>
       <c r="P156" s="2"/>
       <c r="Q156" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
@@ -10698,26 +10698,26 @@
         <v>21</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K157" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L157" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="M157" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="N157" s="2" t="s">
         <v>689</v>
-      </c>
-      <c r="M157" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="N157" s="2" t="s">
-        <v>690</v>
       </c>
       <c r="O157" s="2" t="s">
         <v>85</v>
       </c>
       <c r="P157" s="2"/>
       <c r="Q157" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
@@ -10747,26 +10747,26 @@
         <v>21</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L158" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="M158" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="N158" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="M158" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="N158" s="2" t="s">
+      <c r="O158" s="2" t="s">
         <v>694</v>
-      </c>
-      <c r="O158" s="2" t="s">
-        <v>695</v>
       </c>
       <c r="P158" s="2"/>
       <c r="Q158" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
@@ -10796,26 +10796,26 @@
         <v>21</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K159" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L159" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="N159" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="M159" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="N159" s="2" t="s">
-        <v>699</v>
-      </c>
       <c r="O159" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P159" s="2"/>
       <c r="Q159" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
@@ -10851,16 +10851,16 @@
         <v>37</v>
       </c>
       <c r="L160" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="M160" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="M160" s="2" t="s">
+      <c r="N160" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="O160" s="2" t="s">
         <v>702</v>
-      </c>
-      <c r="N160" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="O160" s="2" t="s">
-        <v>703</v>
       </c>
       <c r="P160" s="2"/>
       <c r="Q160" s="2" t="s">
@@ -10894,26 +10894,26 @@
         <v>21</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K161" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L161" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="M161" s="2" t="s">
         <v>88</v>
       </c>
       <c r="N161" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="O161" s="2" t="s">
         <v>109</v>
       </c>
       <c r="P161" s="2"/>
       <c r="Q161" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
@@ -10943,26 +10943,26 @@
         <v>21</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K162" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L162" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="M162" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="M162" s="2" t="s">
+      <c r="N162" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="N162" s="2" t="s">
+      <c r="O162" s="2" t="s">
         <v>711</v>
-      </c>
-      <c r="O162" s="2" t="s">
-        <v>712</v>
       </c>
       <c r="P162" s="2"/>
       <c r="Q162" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
@@ -10989,7 +10989,7 @@
         <v>20</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="J163" s="2" t="s">
         <v>117</v>
@@ -10998,20 +10998,20 @@
         <v>37</v>
       </c>
       <c r="L163" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="N163" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P163" s="2"/>
       <c r="Q163" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
@@ -11047,20 +11047,20 @@
         <v>31</v>
       </c>
       <c r="L164" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="M164" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="M164" s="2" t="s">
-        <v>718</v>
       </c>
       <c r="N164" s="2" t="s">
         <v>102</v>
       </c>
       <c r="O164" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="P164" s="2"/>
       <c r="Q164" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
@@ -11096,16 +11096,16 @@
         <v>31</v>
       </c>
       <c r="L165" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="M165" s="2" t="s">
         <v>48</v>
       </c>
       <c r="N165" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="O165" s="2" t="s">
         <v>722</v>
-      </c>
-      <c r="O165" s="2" t="s">
-        <v>723</v>
       </c>
       <c r="P165" s="2"/>
       <c r="Q165" s="2" t="s">
@@ -11139,26 +11139,26 @@
         <v>21</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="K166" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L166" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="M166" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="M166" s="2" t="s">
-        <v>726</v>
-      </c>
       <c r="N166" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="O166" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P166" s="2"/>
       <c r="Q166" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
@@ -11185,29 +11185,29 @@
         <v>20</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="K167" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L167" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="M167" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="M167" s="2" t="s">
+      <c r="N167" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="N167" s="2" t="s">
+      <c r="O167" s="2" t="s">
         <v>731</v>
-      </c>
-      <c r="O167" s="2" t="s">
-        <v>732</v>
       </c>
       <c r="P167" s="2"/>
       <c r="Q167" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.2">
@@ -11237,26 +11237,26 @@
         <v>21</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K168" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L168" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="M168" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="M168" s="2" t="s">
+      <c r="N168" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="N168" s="2" t="s">
-        <v>737</v>
-      </c>
       <c r="O168" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P168" s="2"/>
       <c r="Q168" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.2">
@@ -11286,26 +11286,26 @@
         <v>21</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="K169" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L169" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="M169" s="2" t="s">
         <v>33</v>
       </c>
       <c r="N169" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="O169" s="2" t="s">
         <v>741</v>
-      </c>
-      <c r="O169" s="2" t="s">
-        <v>742</v>
       </c>
       <c r="P169" s="2"/>
       <c r="Q169" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.2">
@@ -11335,19 +11335,19 @@
         <v>21</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="K170" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M170" s="2" t="s">
         <v>132</v>
       </c>
       <c r="N170" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="O170" s="2" t="s">
         <v>109</v>
@@ -11384,26 +11384,26 @@
         <v>21</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="K171" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L171" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="M171" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="M171" s="2" t="s">
+      <c r="N171" s="2" t="s">
         <v>747</v>
       </c>
-      <c r="N171" s="2" t="s">
+      <c r="O171" s="2" t="s">
         <v>748</v>
-      </c>
-      <c r="O171" s="2" t="s">
-        <v>749</v>
       </c>
       <c r="P171" s="2"/>
       <c r="Q171" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
@@ -11433,26 +11433,26 @@
         <v>21</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="K172" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L172" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="M172" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="M172" s="2" t="s">
-        <v>753</v>
-      </c>
       <c r="N172" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="O172" s="2" t="s">
         <v>74</v>
       </c>
       <c r="P172" s="2"/>
       <c r="Q172" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
@@ -11482,7 +11482,7 @@
         <v>21</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="K173" s="2" t="s">
         <v>31</v>
@@ -11491,7 +11491,7 @@
         <v>48</v>
       </c>
       <c r="M173" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N173" s="2" t="s">
         <v>185</v>
@@ -11501,7 +11501,7 @@
       </c>
       <c r="P173" s="2"/>
       <c r="Q173" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
@@ -11531,13 +11531,13 @@
         <v>21</v>
       </c>
       <c r="J174" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="K174" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L174" s="2" t="s">
         <v>756</v>
-      </c>
-      <c r="K174" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="L174" s="2" t="s">
-        <v>757</v>
       </c>
       <c r="M174" s="2" t="s">
         <v>137</v>
@@ -11550,7 +11550,7 @@
       </c>
       <c r="P174" s="2"/>
       <c r="Q174" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
@@ -11580,26 +11580,26 @@
         <v>21</v>
       </c>
       <c r="J175" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="K175" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L175" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="M175" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="M175" s="2" t="s">
-        <v>760</v>
-      </c>
       <c r="N175" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O175" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P175" s="2"/>
       <c r="Q175" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -11629,26 +11629,26 @@
         <v>21</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K176" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L176" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="M176" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="M176" s="2" t="s">
+      <c r="N176" s="2" t="s">
         <v>763</v>
-      </c>
-      <c r="N176" s="2" t="s">
-        <v>764</v>
       </c>
       <c r="O176" s="2" t="s">
         <v>188</v>
       </c>
       <c r="P176" s="2"/>
       <c r="Q176" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>